<commit_message>
added speaker class and texture
</commit_message>
<xml_diff>
--- a/resources/coordinate calculator.xlsx
+++ b/resources/coordinate calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Desktop\College Programing\CS-330-Comp-Graphic-and-Visualization\CS-330-3D_Scene\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46B2B99-E2B1-4E06-BB2F-BCE57EE484B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE246AE5-2362-4E37-AD93-19E6064F0EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B07E8EDD-F5E2-4FF6-94E6-76CB92D4814C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>major divisions</t>
   </si>
@@ -72,11 +72,53 @@
   <si>
     <t>y-Coord</t>
   </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>PAINT COORDINATES</t>
+  </si>
+  <si>
+    <t>FLIPPED Y COORDS</t>
+  </si>
+  <si>
+    <t>1 X 1 SCALE COORDS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -121,6 +163,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5BA830-0AFD-498D-906F-EF6ABE7BFF63}">
-  <dimension ref="A2:M56"/>
+  <dimension ref="A2:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,7 +505,9 @@
     <col min="1" max="1" width="13.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="8.88671875" style="3"/>
+    <col min="7" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="10.21875" style="3" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2090,7 +2149,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="49" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G49" s="2">
         <v>11</v>
       </c>
@@ -2114,7 +2173,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="51" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G51" s="2">
         <v>27</v>
       </c>
@@ -2138,7 +2197,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="52" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G52" s="2">
         <v>26</v>
       </c>
@@ -2160,7 +2219,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="53" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G53" s="2">
         <v>10</v>
       </c>
@@ -2184,7 +2243,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="54" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G54" s="2">
         <v>9</v>
       </c>
@@ -2206,7 +2265,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="55" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G55" s="2">
         <v>26</v>
       </c>
@@ -2228,7 +2287,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="56" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G56" s="2">
         <v>10</v>
       </c>
@@ -2252,7 +2311,980 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60" s="5"/>
+      <c r="B60" s="1">
+        <v>3112</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3380</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62"/>
+      <c r="H62" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I62" s="7"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1">
+        <v>970</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1">
+        <f>B64</f>
+        <v>970</v>
+      </c>
+      <c r="F64" s="3">
+        <f>$C$60-C64</f>
+        <v>1680</v>
+      </c>
+      <c r="H64" s="8">
+        <f>E64/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I64" s="8">
+        <f>F64/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1">
+        <f>B65</f>
+        <v>2150</v>
+      </c>
+      <c r="F65" s="3">
+        <f t="shared" ref="F65:F92" si="38">$C$60-C65</f>
+        <v>1680</v>
+      </c>
+      <c r="H65" s="8">
+        <f>E65/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I65" s="8">
+        <f>F65/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A66" s="4">
+        <v>2</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1">
+        <f>B66</f>
+        <v>2150</v>
+      </c>
+      <c r="F66" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H66" s="8">
+        <f>E66/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I66" s="8">
+        <f>F66/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
+        <v>3</v>
+      </c>
+      <c r="B67" s="1">
+        <v>970</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1">
+        <f>B67</f>
+        <v>970</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H67" s="8">
+        <f>E67/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I67" s="8">
+        <f>F67/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="3"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A69" s="4">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1">
+        <v>970</v>
+      </c>
+      <c r="C69" s="1">
+        <v>750</v>
+      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1">
+        <f>B69</f>
+        <v>970</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="38"/>
+        <v>2630</v>
+      </c>
+      <c r="H69" s="8">
+        <f>E69/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I69" s="8">
+        <f>F69/$C$60</f>
+        <v>0.77810650887573962</v>
+      </c>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A70" s="4">
+        <v>5</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C70" s="1">
+        <v>750</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1">
+        <f>B70</f>
+        <v>2150</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="38"/>
+        <v>2630</v>
+      </c>
+      <c r="H70" s="8">
+        <f>E70/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I70" s="8">
+        <f>F70/$C$60</f>
+        <v>0.77810650887573962</v>
+      </c>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1">
+        <v>970</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1">
+        <f>B71</f>
+        <v>970</v>
+      </c>
+      <c r="F71" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H71" s="8">
+        <f>E71/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I71" s="8">
+        <f>F71/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
+        <v>1</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1">
+        <f>B72</f>
+        <v>2150</v>
+      </c>
+      <c r="F72" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H72" s="8">
+        <f>E72/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I72" s="8">
+        <f>F72/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="3"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74" s="5">
+        <v>7</v>
+      </c>
+      <c r="B74" s="1">
+        <v>970</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1">
+        <f>B74</f>
+        <v>970</v>
+      </c>
+      <c r="F74" s="3">
+        <f t="shared" si="38"/>
+        <v>3380</v>
+      </c>
+      <c r="H74" s="8">
+        <f>E74/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I74" s="8">
+        <f>F74/$C$60</f>
+        <v>1</v>
+      </c>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" s="5">
+        <v>6</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1">
+        <f>B75</f>
+        <v>2150</v>
+      </c>
+      <c r="F75" s="3">
+        <f t="shared" si="38"/>
+        <v>3380</v>
+      </c>
+      <c r="H75" s="8">
+        <f>E75/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I75" s="8">
+        <f>F75/$C$60</f>
+        <v>1</v>
+      </c>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A76" s="5">
+        <v>4</v>
+      </c>
+      <c r="B76" s="1">
+        <v>970</v>
+      </c>
+      <c r="C76" s="1">
+        <v>750</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1">
+        <f>B76</f>
+        <v>970</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" si="38"/>
+        <v>2630</v>
+      </c>
+      <c r="H76" s="8">
+        <f>E76/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I76" s="8">
+        <f>F76/$C$60</f>
+        <v>0.77810650887573962</v>
+      </c>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C77" s="1">
+        <v>750</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1">
+        <f>B77</f>
+        <v>2150</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="38"/>
+        <v>2630</v>
+      </c>
+      <c r="H77" s="8">
+        <f>E77/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I77" s="8">
+        <f>F77/$C$60</f>
+        <v>0.77810650887573962</v>
+      </c>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="3"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79" s="5">
+        <v>3</v>
+      </c>
+      <c r="B79" s="1">
+        <v>970</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1">
+        <f>B79</f>
+        <v>970</v>
+      </c>
+      <c r="F79" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H79" s="8">
+        <f>E79/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I79" s="8">
+        <f>F79/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" s="5">
+        <v>2</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1">
+        <f>B80</f>
+        <v>2150</v>
+      </c>
+      <c r="F80" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H80" s="8">
+        <f>E80/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I80" s="8">
+        <f>F80/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>7</v>
+      </c>
+      <c r="B81" s="1">
+        <v>970</v>
+      </c>
+      <c r="C81" s="1">
+        <v>3380</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1">
+        <f>B81</f>
+        <v>970</v>
+      </c>
+      <c r="F81" s="3">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H81" s="8">
+        <f>E81/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I81" s="8">
+        <f>F81/$C$60</f>
+        <v>0</v>
+      </c>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82" s="5">
+        <v>6</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3380</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1">
+        <f>B82</f>
+        <v>2150</v>
+      </c>
+      <c r="F82" s="3">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H82" s="8">
+        <f>E82/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I82" s="8">
+        <f>F82/$C$60</f>
+        <v>0</v>
+      </c>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="3"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A84" s="5">
+        <v>4</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <f>B84</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H84" s="8">
+        <f>E84/$B$60</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="8">
+        <f>F84/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85" s="5">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1">
+        <v>970</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1">
+        <f>B85</f>
+        <v>970</v>
+      </c>
+      <c r="F85" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H85" s="8">
+        <f>E85/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I85" s="8">
+        <f>F85/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86" s="5">
+        <v>7</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1">
+        <f>B86</f>
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H86" s="8">
+        <f>E86/$B$60</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="8">
+        <f>F86/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="5">
+        <v>3</v>
+      </c>
+      <c r="B87" s="1">
+        <v>970</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1">
+        <f>B87</f>
+        <v>970</v>
+      </c>
+      <c r="F87" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H87" s="8">
+        <f>E87/$B$60</f>
+        <v>0.31169665809768637</v>
+      </c>
+      <c r="I87" s="8">
+        <f>F87/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="3"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" s="5">
+        <v>1</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1">
+        <f>B89</f>
+        <v>2150</v>
+      </c>
+      <c r="F89" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H89" s="8">
+        <f>E89/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I89" s="8">
+        <f>F89/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
+        <v>5</v>
+      </c>
+      <c r="B90" s="1">
+        <v>3110</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1700</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1">
+        <f>B90</f>
+        <v>3110</v>
+      </c>
+      <c r="F90" s="3">
+        <f t="shared" si="38"/>
+        <v>1680</v>
+      </c>
+      <c r="H90" s="8">
+        <f>E90/$B$60</f>
+        <v>0.99935732647814912</v>
+      </c>
+      <c r="I90" s="8">
+        <f>F90/$C$60</f>
+        <v>0.49704142011834318</v>
+      </c>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
+        <v>6</v>
+      </c>
+      <c r="B91" s="1">
+        <v>3110</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1">
+        <f>B91</f>
+        <v>3110</v>
+      </c>
+      <c r="F91" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H91" s="8">
+        <f>E91/$B$60</f>
+        <v>0.99935732647814912</v>
+      </c>
+      <c r="I91" s="8">
+        <f>F91/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2430</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1">
+        <f>B92</f>
+        <v>2150</v>
+      </c>
+      <c r="F92" s="3">
+        <f t="shared" si="38"/>
+        <v>950</v>
+      </c>
+      <c r="H92" s="8">
+        <f>E92/$B$60</f>
+        <v>0.69087403598971719</v>
+      </c>
+      <c r="I92" s="8">
+        <f>F92/$C$60</f>
+        <v>0.28106508875739644</v>
+      </c>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93" s="5"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94" s="5"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95" s="5"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A96" s="5"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="5"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="5"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="5"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="5"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="5"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="5"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="5"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="5"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="5"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="5"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="5"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="5"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="5"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="5"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="5"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="5"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="5"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="5"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="5"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="5"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="5"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="5"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="5"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="H62:I62"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>